<commit_message>
proste je to ted lepsi
</commit_message>
<xml_diff>
--- a/funcni data set - Copy.xlsx
+++ b/funcni data set - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f619c9dbaff66258/development/github/sws/code/predictive modeling/funkcni/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f619c9dbaff66258/Dokumenty/GitHub/predikce-nabidky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{7CD2E4E8-1F28-44FE-ADE5-F3B50EE5FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F41AF642-3A87-400A-B926-C397245051B5}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{7CD2E4E8-1F28-44FE-ADE5-F3B50EE5FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{296F365B-72D8-492D-B6C0-41E421DB72D5}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>datum</t>
   </si>
@@ -314,6 +314,9 @@
   <si>
     <t>mesicu</t>
   </si>
+  <si>
+    <t>datetime</t>
+  </si>
 </sst>
 </file>
 
@@ -551,10 +554,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -856,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DC190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA28" workbookViewId="0">
-      <selection activeCell="CB106" sqref="CB106"/>
+    <sheetView tabSelected="1" topLeftCell="CH1" workbookViewId="0">
+      <selection activeCell="CQ2" sqref="CQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +872,7 @@
     <col min="81" max="81" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1152,11 @@
       <c r="CP1" t="s">
         <v>78</v>
       </c>
+      <c r="CQ1" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>201502</v>
       </c>
@@ -1216,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>201503</v>
       </c>
@@ -1518,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>201504</v>
       </c>
@@ -1820,7 +1822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>201505</v>
       </c>
@@ -2178,7 +2180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>201506</v>
       </c>
@@ -2536,7 +2538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>201507</v>
       </c>
@@ -2894,7 +2896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>201508</v>
       </c>
@@ -3252,7 +3254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>201509</v>
       </c>
@@ -3610,7 +3612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>201510</v>
       </c>
@@ -3968,7 +3970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>201511</v>
       </c>
@@ -4326,7 +4328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>201512</v>
       </c>
@@ -4684,7 +4686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>201601</v>
       </c>
@@ -5042,7 +5044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>201602</v>
       </c>
@@ -5400,7 +5402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>201603</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>201604</v>
       </c>
@@ -25390,7 +25392,7 @@
         <v>64</v>
       </c>
       <c r="CB70">
-        <f t="shared" ref="CB70:CB98" si="56">IF(CD70&gt;75,3,IF(CD70&lt;45,1,2))</f>
+        <f t="shared" ref="CB70:CB97" si="56">IF(CD70&gt;75,3,IF(CD70&lt;45,1,2))</f>
         <v>3</v>
       </c>
       <c r="CC70" s="8">

</xml_diff>